<commit_message>
added debug variable, updated model with launcherbasedimport
</commit_message>
<xml_diff>
--- a/Raw tables/workcenters.xlsx
+++ b/Raw tables/workcenters.xlsx
@@ -458,17 +458,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>20004</t>
+          <t>20002</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>40402</t>
+          <t>54201</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>LINE 2 DRY EXTR HAZLETON</t>
+          <t>BAKE SYSTEM 1 (WEST) OGDEN</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -480,44 +480,44 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>20001</t>
+          <t>20002</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>34101</t>
+          <t>54202</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>X185 SLURRY LINE BERN</t>
+          <t>BAKE SYSTEM 2 (MIDDLE) OGDEN</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>SLURR</t>
+          <t>EXTR</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>20001</t>
+          <t>20002</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>34102</t>
+          <t>54203</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>C2 SLURRY LINE BERN</t>
+          <t>BAKE SYSTEM 3 (EAST) OGDENT</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>SLURR</t>
+          <t>EXTR</t>
         </is>
       </c>
     </row>
@@ -529,325 +529,325 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>34201</t>
+          <t>64201</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>DRY SLURRY EAST OGDEN</t>
+          <t>CAN PROCESSING OGDEN</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>SLURR</t>
+          <t>EXTR</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>20002</t>
+          <t>10001</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>34202</t>
+          <t>72101</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>SLURRY WEST OGDEN</t>
+          <t>BAG LINE - BERN</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>SLURR</t>
+          <t>PACK</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>20004</t>
+          <t>10001</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>34401</t>
+          <t>72102</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>SLURRY LINE 1 HAZLETON</t>
+          <t>TOTE LINE BERN</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>SLURR</t>
+          <t>PACK</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>20004</t>
+          <t>20001</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>34402</t>
+          <t>74101</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>SLURRY LINE 2 HAZLETON</t>
+          <t>BEMIS 1 BERN</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>SLURR</t>
+          <t>PACK</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>20005</t>
+          <t>20001</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>34501</t>
+          <t>74102</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>SLURRY X185 PAWNEE CITY</t>
+          <t>BEMIS 2 BERN</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>SLURR</t>
+          <t>PACK</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>20002</t>
+          <t>20001</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>35201</t>
+          <t>74103</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>SLURRY BAKED OGDEN</t>
+          <t>PARSONS BERN</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>SLURR</t>
+          <t>PACK</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>10001</t>
+          <t>20001</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>21101</t>
+          <t>74104</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>MIXER LANI BERN</t>
+          <t>JEM LINE 5 BERN</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>MILL</t>
+          <t>PACK</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>10001</t>
+          <t>20001</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>21102</t>
+          <t>74105</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>GRINDER #1 BERN</t>
+          <t>JEM LINE 6 BERN</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>MILL</t>
+          <t>PACK</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>10001</t>
+          <t>20001</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>21103</t>
+          <t>74106</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>GRINDER #2 BERN</t>
+          <t>TOTE BAG LINE BERN</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>MILL</t>
+          <t>PACK</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>10002</t>
+          <t>20002</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>21201</t>
+          <t>74201</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>MIXER BROWNWOOD</t>
+          <t>LINE 1 LARGE MANUAL LINE OGDEN</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>MILL</t>
+          <t>PACK</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>10002</t>
+          <t>20002</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>21202</t>
+          <t>74202</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>GRINDER #1 BROWNWOOD</t>
+          <t>LINE 2 LARGE AUTO OGDEN</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>MILL</t>
+          <t>PACK</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>20001</t>
+          <t>20002</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>40101</t>
+          <t>74203</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>C2 EXTRUDER BERN</t>
+          <t>LINE 3 SMALL LINE OGDEN</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>EXTR</t>
+          <t>PACK</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>20001</t>
+          <t>20003</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>40102</t>
+          <t>74301</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>X185 EXTRUDER BERN</t>
+          <t>DRY PACK NORTH LARGE WOODLAND</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>EXTR</t>
+          <t>PACK</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>20002</t>
+          <t>20003</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>40201</t>
+          <t>74302</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>WEST DRY EXTRUSION OGDEN</t>
+          <t>DRY PACK SOUTH LARGE WOODLAND</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>EXTR</t>
+          <t>PACK</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>20002</t>
+          <t>20003</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>40202</t>
+          <t>74303</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>EAST DRY EXTRUSION OGDEN</t>
+          <t>DRY PACK SMALL WOODLAND</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>EXTR</t>
+          <t>PACK</t>
         </is>
       </c>
     </row>
@@ -859,39 +859,39 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>40301</t>
+          <t>74304</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>NORTH DRY EXTR WOODLAND</t>
+          <t>DRY PACK OLD SMALL WOODLAND</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>EXTR</t>
+          <t>PACK</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20003</t>
+          <t>20004</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>40302</t>
+          <t>74401</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>SOUTH DRY EXTR WOODLAND</t>
+          <t>LINE 1 LARGE HAZLETON</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>EXTR</t>
+          <t>PACK</t>
         </is>
       </c>
     </row>
@@ -903,100 +903,100 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>40401</t>
+          <t>74402</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>LINE #1 DRY EXTR HAZELTON</t>
+          <t>LINE 2 HAND FILL HAZLETON</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>EXTR</t>
+          <t>PACK</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>20005</t>
+          <t>20004</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>40501</t>
+          <t>74403</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>X165 EXTRUDER PAWNEE CITY</t>
+          <t>LINE 3 SMALL HAZLETON</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>EXTR</t>
+          <t>PACK</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>20005</t>
+          <t>20004</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>40502</t>
+          <t>74404</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>X185 EXTRUDER PAWNEE CITY</t>
+          <t>LINE 4 LARGE HAZELTON</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>EXTR</t>
+          <t>PACK</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>20006</t>
+          <t>20004</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>40601</t>
+          <t>74405</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>E750 EXTRUDER BAXTER SPRINGS</t>
+          <t>LINE 5 POUCHER HAZLETON</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>EXTR</t>
+          <t>PACK</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>20002</t>
+          <t>20006</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>54201</t>
+          <t>40601</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>BAKE SYSTEM 1 (WEST) OGDEN</t>
+          <t>E750 EXTRUDER BAXTER SPRINGS</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1008,17 +1008,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>20002</t>
+          <t>20005</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>54202</t>
+          <t>40502</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>BAKE SYSTEM 2 (MIDDLE) OGDEN</t>
+          <t>X185 EXTRUDER PAWNEE CITY</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1030,17 +1030,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>20002</t>
+          <t>20005</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>54203</t>
+          <t>40501</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>BAKE SYSTEM 3 (EAST) OGDENT</t>
+          <t>X165 EXTRUDER PAWNEE CITY</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1052,17 +1052,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>20002</t>
+          <t>20004</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>64201</t>
+          <t>40401</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>CAN PROCESSING OGDEN</t>
+          <t>LINE #1 DRY EXTR HAZELTON</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1074,88 +1074,88 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>10001</t>
+          <t>20003</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>72101</t>
+          <t>40302</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>BAG LINE - BERN</t>
+          <t>SOUTH DRY EXTR WOODLAND</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>PACK</t>
+          <t>EXTR</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>10001</t>
+          <t>20003</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>72102</t>
+          <t>40301</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>TOTE LINE BERN</t>
+          <t>NORTH DRY EXTR WOODLAND</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>PACK</t>
+          <t>EXTR</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>20001</t>
+          <t>20002</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>74101</t>
+          <t>40202</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>BEMIS 1 BERN</t>
+          <t>EAST DRY EXTRUSION OGDEN</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>PACK</t>
+          <t>EXTR</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>20001</t>
+          <t>20002</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>74102</t>
+          <t>40201</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>BEMIS 2 BERN</t>
+          <t>WEST DRY EXTRUSION OGDEN</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>PACK</t>
+          <t>EXTR</t>
         </is>
       </c>
     </row>
@@ -1167,17 +1167,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>74103</t>
+          <t>40102</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>PARSONS BERN</t>
+          <t>X185 EXTRUDER BERN</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>PACK</t>
+          <t>EXTR</t>
         </is>
       </c>
     </row>
@@ -1189,320 +1189,320 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>74104</t>
+          <t>40101</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>JEM LINE 5 BERN</t>
+          <t>C2 EXTRUDER BERN</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>PACK</t>
+          <t>EXTR</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>20001</t>
+          <t>10002</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>74105</t>
+          <t>21202</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>JEM LINE 6 BERN</t>
+          <t>GRINDER #1 BROWNWOOD</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>PACK</t>
+          <t>MILL</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>20001</t>
+          <t>10002</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>74106</t>
+          <t>21201</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>TOTE BAG LINE BERN</t>
+          <t>MIXER BROWNWOOD</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>PACK</t>
+          <t>MILL</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>20002</t>
+          <t>10001</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>74201</t>
+          <t>21103</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>LINE 1 LARGE MANUAL LINE OGDEN</t>
+          <t>GRINDER #2 BERN</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>PACK</t>
+          <t>MILL</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>20002</t>
+          <t>10001</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>74202</t>
+          <t>21102</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>LINE 2 LARGE AUTO OGDEN</t>
+          <t>GRINDER #1 BERN</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>PACK</t>
+          <t>MILL</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>20002</t>
+          <t>10001</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>74203</t>
+          <t>21101</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>LINE 3 SMALL LINE OGDEN</t>
+          <t>MIXER LANI BERN</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>PACK</t>
+          <t>MILL</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>20003</t>
+          <t>20002</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>74301</t>
+          <t>35201</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>DRY PACK NORTH LARGE WOODLAND</t>
+          <t>SLURRY BAKED OGDEN</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>PACK</t>
+          <t>SLURR</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>20003</t>
+          <t>20005</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>74302</t>
+          <t>34501</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>DRY PACK SOUTH LARGE WOODLAND</t>
+          <t>SLURRY X185 PAWNEE CITY</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>PACK</t>
+          <t>SLURR</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>20003</t>
+          <t>20004</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>74303</t>
+          <t>34402</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>DRY PACK SMALL WOODLAND</t>
+          <t>SLURRY LINE 2 HAZLETON</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>PACK</t>
+          <t>SLURR</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>20003</t>
+          <t>20004</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>74304</t>
+          <t>34401</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>DRY PACK OLD SMALL WOODLAND</t>
+          <t>SLURRY LINE 1 HAZLETON</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>PACK</t>
+          <t>SLURR</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>20004</t>
+          <t>20002</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>74401</t>
+          <t>34202</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>LINE 1 LARGE HAZLETON</t>
+          <t>SLURRY WEST OGDEN</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>PACK</t>
+          <t>SLURR</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>20004</t>
+          <t>20002</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>74402</t>
+          <t>34201</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>LINE 2 HAND FILL HAZLETON</t>
+          <t>DRY SLURRY EAST OGDEN</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>PACK</t>
+          <t>SLURR</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>20004</t>
+          <t>20001</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>74403</t>
+          <t>34102</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>LINE 3 SMALL HAZLETON</t>
+          <t>C2 SLURRY LINE BERN</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>PACK</t>
+          <t>SLURR</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>20004</t>
+          <t>20001</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>74404</t>
+          <t>34101</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>LINE 4 LARGE HAZELTON</t>
+          <t>X185 SLURRY LINE BERN</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>PACK</t>
+          <t>SLURR</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>20004</t>
+          <t>10002</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>74405</t>
+          <t>72201</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>LINE 5 POUCHER HAZLETON</t>
+          <t>TOTE LINE BROWNWOOD</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1519,34 +1519,34 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>74406</t>
+          <t>40402</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>LINE 6 SMALL HAZLETON</t>
+          <t>LINE 2 DRY EXTR HAZLETON</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>PACK</t>
+          <t>EXTR</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>20005</t>
+          <t>20004</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>74501</t>
+          <t>74406</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>X165 PACKAGING LINE PAWNEE CIT</t>
+          <t>LINE 6 SMALL HAZLETON</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1563,12 +1563,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>74502</t>
+          <t>74501</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>UVA PAWNEE CITY</t>
+          <t>X165 PACKAGING LINE PAWNEE CIT</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1585,12 +1585,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>74503</t>
+          <t>74502</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>JEM PAWNEE CITY</t>
+          <t>UVA PAWNEE CITY</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1607,12 +1607,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>74504</t>
+          <t>74503</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>SAMPLE LINE PAWNEE CITY</t>
+          <t>JEM PAWNEE CITY</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1629,12 +1629,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>74505</t>
+          <t>74504</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>JEM #2 PAWNEE CITY</t>
+          <t>SAMPLE LINE PAWNEE CITY</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1651,12 +1651,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>74506</t>
+          <t>74505</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>X165 TOTE BAG LINE PAWNEE CITY</t>
+          <t>JEM #2 PAWNEE CITY</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1673,12 +1673,12 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>74507</t>
+          <t>74506</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>PARSONS PAWNEE CITY</t>
+          <t>X165 TOTE BAG LINE PAWNEE CITY</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1695,12 +1695,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>74508</t>
+          <t>74507</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>BEMIS PAWNEE CITY</t>
+          <t>PARSONS PAWNEE CITY</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1717,12 +1717,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>74509</t>
+          <t>74508</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>X185 TOTE BAG LINE PAWNEE CITY</t>
+          <t>BEMIS PAWNEE CITY</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1734,17 +1734,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>20006</t>
+          <t>20005</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>74601</t>
+          <t>74509</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>BAXTER BIG BAG - LINE 2</t>
+          <t>X185 TOTE BAG LINE PAWNEE CITY</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1761,12 +1761,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>74602</t>
+          <t>74601</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>BAXTER SMALL BAG -  LINE 1</t>
+          <t>BAXTER BIG BAG - LINE 2</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -1778,17 +1778,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>20002</t>
+          <t>20006</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>75201</t>
+          <t>74602</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>BAKE PACK LINE 1 OGDEN</t>
+          <t>BAXTER SMALL BAG -  LINE 1</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -1805,12 +1805,12 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>75202</t>
+          <t>75201</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>BAKE PACK LINE 2 OGDEN</t>
+          <t>BAKE PACK LINE 1 OGDEN</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -1827,12 +1827,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>75203</t>
+          <t>75202</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>BAKE PACK LINE 3 OGDEN</t>
+          <t>BAKE PACK LINE 2 OGDEN</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -1849,12 +1849,12 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>75204</t>
+          <t>75203</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>BAKE PACK LINE 4 OGDEN</t>
+          <t>BAKE PACK LINE 3 OGDEN</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -1871,12 +1871,12 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>75205</t>
+          <t>75204</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>BAKE PACK LINE 5 OGDEN</t>
+          <t>BAKE PACK LINE 4 OGDEN</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -1893,12 +1893,12 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>75206</t>
+          <t>75205</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>BAKE PACK ROBOT OGDEN</t>
+          <t>BAKE PACK LINE 5 OGDEN</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -1915,12 +1915,12 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>75207</t>
+          <t>75206</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>BAKE PACK HANDPACK OGDEN</t>
+          <t>BAKE PACK ROBOT OGDEN</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -1937,12 +1937,12 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>76201</t>
+          <t>75207</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>CAN PACKAGING OGDEN</t>
+          <t>BAKE PACK HANDPACK OGDEN</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -1959,12 +1959,12 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>76202</t>
+          <t>76201</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>CAN VARIETY PACK OGDEN</t>
+          <t>CAN PACKAGING OGDEN</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -1976,17 +1976,17 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>20005</t>
+          <t>20002</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>74510</t>
+          <t>76202</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>SUP PAWNEE CITY</t>
+          <t>CAN VARIETY PACK OGDEN</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2003,12 +2003,12 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>74511</t>
+          <t>74510</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>PSGLEE PAWNEE CITY</t>
+          <t>SUP PAWNEE CITY</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2020,17 +2020,17 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>10002</t>
+          <t>20005</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>72201</t>
+          <t>74511</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>TOTE LINE BROWNWOOD</t>
+          <t>PSGLEE PAWNEE CITY</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">

</xml_diff>